<commit_message>
add type content slide
</commit_message>
<xml_diff>
--- a/components/mockup-data/data/slideType.xlsx
+++ b/components/mockup-data/data/slideType.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dhieu\Learn\Học kì VII\Web\Kahoot\BE\components\mockup-data\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B00F4D0-0E40-4C44-AB49-4566D41C6F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B3CD2E-C114-4DEB-8BCA-FC78BB76424E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2976" yWindow="1728" windowWidth="19224" windowHeight="10056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>parent_type_id</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>Multiple Choice</t>
+  </si>
+  <si>
+    <t>Heading</t>
+  </si>
+  <si>
+    <t>Paragraph</t>
   </si>
 </sst>
 </file>
@@ -351,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -378,6 +384,22 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>